<commit_message>
planeacion general del proyecto
</commit_message>
<xml_diff>
--- a/Documentacion/planeación.xlsx
+++ b/Documentacion/planeación.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proyectoFinal\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Etapas</t>
   </si>
@@ -25,9 +30,6 @@
   </si>
   <si>
     <t>Requisitos</t>
-  </si>
-  <si>
-    <t>Runcionales y no funcionales</t>
   </si>
   <si>
     <t>Análisis y diseño</t>
@@ -137,13 +139,16 @@
       <t xml:space="preserve"> Días</t>
     </r>
   </si>
+  <si>
+    <t>Funcionales y no funcionales</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -295,25 +300,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,6 +329,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -371,7 +380,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,7 +415,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -618,7 +627,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,70 +647,70 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="3">
         <v>42191</v>
       </c>
@@ -744,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -759,7 +768,7 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
@@ -777,11 +786,11 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -796,7 +805,7 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -813,11 +822,11 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -832,13 +841,15 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -851,14 +862,16 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -870,15 +883,15 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -891,7 +904,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -908,16 +921,16 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -929,40 +942,38 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -974,16 +985,16 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -997,7 +1008,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>